<commit_message>
Added historical data storage for composite model (v0.20)
</commit_message>
<xml_diff>
--- a/deployment/forecast-tables.xlsx
+++ b/deployment/forecast-tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\modules\create-sql-tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF208A75-1D48-483A-873B-0E2345977F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC88B6D2-7498-448C-829B-9EC1F76E0DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="forecasts" sheetId="12" r:id="rId1"/>
@@ -1685,34 +1685,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1944,6 +1916,34 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1969,24 +1969,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:L114" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9BF0F429-29B2-4294-B7A2-79B0C1D59CBE}" name="Table1327" displayName="Table1327" ref="A1:L114" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L114" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L113">
     <sortCondition ref="C1:C113"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="14"/>
-    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="13"/>
-    <tableColumn id="21" xr3:uid="{621C897B-D737-4C13-BA42-A8685BC996AF}" name="disporder" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="release" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="9"/>
-    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{1C3AA07F-56DA-4994-9225-B9D5205877C4}" name="hist_source" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{167E969F-257F-4290-9851-386858BC28D6}" name="hist_source_key" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{A6782029-125F-4B9D-98E4-9AFC08718DFD}" name="hist_source_freq" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{E7C5D4F8-69B1-411D-884E-EB9AB632410B}" name="hist_source_transform" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{06A4A672-09EE-4DC6-9B74-6C96B10B19A9}" name="varname" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{9EE4570B-6B9A-4A19-BCD2-CC9F558F1A39}" name="fullname" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{445818A7-0C03-496A-9F03-C0F1A692B978}" name="dispgroup" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{621C897B-D737-4C13-BA42-A8685BC996AF}" name="disporder" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{C16CDFB6-0351-4C97-BE71-77D64AA5A8C9}" name="release" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{1D18F3A6-5B37-4AE0-A67A-4BAEED08A5F9}" name="units" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{65521ED0-11BE-4DE7-8954-09B7C6A08CC0}" name="d1" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{9D56F00C-543D-43DE-9916-EE4811ABA79E}" name="d2" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1C3AA07F-56DA-4994-9225-B9D5205877C4}" name="hist_source" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{167E969F-257F-4290-9851-386858BC28D6}" name="hist_source_key" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A6782029-125F-4B9D-98E4-9AFC08718DFD}" name="hist_source_freq" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{E7C5D4F8-69B1-411D-884E-EB9AB632410B}" name="hist_source_transform" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2464,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C376F7-1E7E-44FE-9F6F-977B435E0AEC}">
   <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4856,7 +4856,7 @@
         <v>420</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>28</v>
+        <v>264</v>
       </c>
       <c r="L64" s="5" t="s">
         <v>231</v>
@@ -6615,16 +6615,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="3" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added description text to forecast fields for use on website (v0.20)
</commit_message>
<xml_diff>
--- a/deployment/forecast-tables.xlsx
+++ b/deployment/forecast-tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D6D3CD-192A-4296-AB44-B5B6F962B8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77AC4F0-F943-4DF1-AE4B-8D4EEA2ECA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="forecasts" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="483">
   <si>
     <t>gdp</t>
   </si>
@@ -1469,6 +1469,21 @@
   </si>
   <si>
     <t>CPIAUCSL</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Fannie Mae's &lt;a href="https://www.fanniemae.com/research-and-insights/forecast"&gt;Economic &amp;amp; Housing Outlook&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>The Philadelphia Federal Reserve's &lt;a href="https://www.philadelphiafed.org/surveys-and-data/real-time-data-research/survey-of-professional-forecasters"&gt;Survey of Professional Forecasters&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>The U.S. Congressional Budget Office's &lt;a href="https://www.cbo.gov/data/budget-economic-data"&gt;10-Year Economic Projections&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>The Wall Street Journal Economic Survey</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1563,6 +1578,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2172,10 +2190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1299AB-5478-4000-9ACB-E921592DFFDD}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,9 +2201,10 @@
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="6" max="6" width="181.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>439</v>
       </c>
@@ -2201,8 +2220,11 @@
       <c r="E1" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>433</v>
       </c>
@@ -2219,7 +2241,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>463</v>
       </c>
@@ -2236,7 +2258,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>461</v>
       </c>
@@ -2253,7 +2275,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>444</v>
       </c>
@@ -2267,10 +2289,13 @@
         <v>437</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F5" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>445</v>
       </c>
@@ -2281,13 +2306,14 @@
         <v>452</v>
       </c>
       <c r="D6" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>446</v>
       </c>
@@ -2301,10 +2327,13 @@
         <v>437</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F7" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>447</v>
       </c>
@@ -2318,10 +2347,13 @@
         <v>437</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F8" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>448</v>
       </c>
@@ -2335,7 +2367,10 @@
         <v>437</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>257</v>
+      </c>
+      <c r="F9" t="s">
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -2347,8 +2382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C376F7-1E7E-44FE-9F6F-977B435E0AEC}">
   <dimension ref="A1:L107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="J64" sqref="J64"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6279,7 +6314,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>